<commit_message>
Updated the excel sheet with 2nd tab in it
</commit_message>
<xml_diff>
--- a/cidr_ranges.xlsx
+++ b/cidr_ranges.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2VPC" sheetId="1" r:id="rId1"/>
+    <sheet name="1 VPC" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
   <si>
     <t>first IP</t>
   </si>
@@ -138,6 +139,27 @@
   </si>
   <si>
     <t>CIDR Range - 10.48.160.0/25</t>
+  </si>
+  <si>
+    <t>10.48.160.0/25</t>
+  </si>
+  <si>
+    <t>10.48.160.0/27</t>
+  </si>
+  <si>
+    <t>10.48.160.32/27</t>
+  </si>
+  <si>
+    <t>10.48.160.64/27</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10.48.160.64</t>
+  </si>
+  <si>
+    <t>10.48.160.96/27</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10.48.160.96</t>
   </si>
 </sst>
 </file>
@@ -477,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="A2:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -691,4 +713,147 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B9:D9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>